<commit_message>
filters track, grade lvl, and prerequisites
</commit_message>
<xml_diff>
--- a/src/main/model/CoursesFinal.xlsx
+++ b/src/main/model/CoursesFinal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fence\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6ad593f627d6d819/Documents/GitHub/CoursesSummative/src/main/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21CFDC65-F467-4810-AA5B-460F14DB8EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{3485982D-FFD1-467E-B4CD-065C9D28A493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1970" yWindow="2680" windowWidth="19200" windowHeight="11170" xr2:uid="{4B1F999D-2B31-4EBB-86BB-F68812B9D625}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4B1F999D-2B31-4EBB-86BB-F68812B9D625}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1438,25 +1438,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D51743-F100-4C15-8601-ED56FE5360A4}">
   <dimension ref="A1:T264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="G96" sqref="G96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.36328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.54296875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.453125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="18.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -1486,7 +1486,7 @@
       <c r="K1"/>
       <c r="L1"/>
     </row>
-    <row r="2" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -1516,7 +1516,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -1546,7 +1546,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" ht="116" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1576,7 +1576,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" ht="116" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1606,7 +1606,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -1636,7 +1636,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1666,7 +1666,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1696,7 +1696,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1726,7 +1726,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -1756,7 +1756,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -1786,7 +1786,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -1816,7 +1816,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
@@ -1846,7 +1846,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
@@ -1876,7 +1876,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>54</v>
       </c>
@@ -1906,7 +1906,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>57</v>
       </c>
@@ -1936,7 +1936,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>59</v>
       </c>
@@ -1966,7 +1966,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>60</v>
       </c>
@@ -1996,7 +1996,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>61</v>
       </c>
@@ -2026,7 +2026,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>65</v>
       </c>
@@ -2056,7 +2056,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>68</v>
       </c>
@@ -2086,7 +2086,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>72</v>
       </c>
@@ -2116,7 +2116,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>75</v>
       </c>
@@ -2146,7 +2146,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>78</v>
       </c>
@@ -2176,7 +2176,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>79</v>
       </c>
@@ -2206,7 +2206,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>80</v>
       </c>
@@ -2236,7 +2236,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
@@ -2266,7 +2266,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>84</v>
       </c>
@@ -2296,7 +2296,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>85</v>
       </c>
@@ -2326,7 +2326,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>88</v>
       </c>
@@ -2356,7 +2356,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>89</v>
       </c>
@@ -2386,7 +2386,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>90</v>
       </c>
@@ -2416,7 +2416,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>93</v>
       </c>
@@ -2446,7 +2446,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>94</v>
       </c>
@@ -2476,7 +2476,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>97</v>
       </c>
@@ -2506,7 +2506,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>101</v>
       </c>
@@ -2536,7 +2536,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>104</v>
       </c>
@@ -2566,7 +2566,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>106</v>
       </c>
@@ -2596,7 +2596,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>107</v>
       </c>
@@ -2626,7 +2626,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>110</v>
       </c>
@@ -2656,7 +2656,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>113</v>
       </c>
@@ -2686,7 +2686,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>116</v>
       </c>
@@ -2716,7 +2716,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>119</v>
       </c>
@@ -2746,7 +2746,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>122</v>
       </c>
@@ -2776,7 +2776,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>129</v>
       </c>
@@ -2806,7 +2806,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>131</v>
       </c>
@@ -2836,7 +2836,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:12" ht="174" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>132</v>
       </c>
@@ -2866,7 +2866,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" ht="174" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>134</v>
       </c>
@@ -2896,7 +2896,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>135</v>
       </c>
@@ -2926,7 +2926,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>137</v>
       </c>
@@ -2956,7 +2956,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:12" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>138</v>
       </c>
@@ -2986,7 +2986,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="1:12" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>139</v>
       </c>
@@ -3016,7 +3016,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>140</v>
       </c>
@@ -3046,7 +3046,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>145</v>
       </c>
@@ -3076,7 +3076,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>144</v>
       </c>
@@ -3106,7 +3106,7 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>146</v>
       </c>
@@ -3136,7 +3136,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>151</v>
       </c>
@@ -3166,7 +3166,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>153</v>
       </c>
@@ -3196,7 +3196,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>155</v>
       </c>
@@ -3223,7 +3223,7 @@
       </c>
       <c r="J59" s="5"/>
     </row>
-    <row r="60" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>158</v>
       </c>
@@ -3250,7 +3250,7 @@
       </c>
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>160</v>
       </c>
@@ -3277,7 +3277,7 @@
       </c>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>162</v>
       </c>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" spans="1:12" ht="116" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>164</v>
       </c>
@@ -3331,7 +3331,7 @@
       </c>
       <c r="J63" s="5"/>
     </row>
-    <row r="64" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>166</v>
       </c>
@@ -3358,7 +3358,7 @@
       </c>
       <c r="J64" s="5"/>
     </row>
-    <row r="65" spans="1:20" ht="87" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" ht="120" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>169</v>
       </c>
@@ -3385,7 +3385,7 @@
       </c>
       <c r="J65" s="5"/>
     </row>
-    <row r="66" spans="1:20" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:20" ht="135" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>171</v>
       </c>
@@ -3412,7 +3412,7 @@
       </c>
       <c r="J66" s="5"/>
     </row>
-    <row r="67" spans="1:20" ht="87" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:20" ht="135" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>174</v>
       </c>
@@ -3439,7 +3439,7 @@
       </c>
       <c r="J67" s="5"/>
     </row>
-    <row r="68" spans="1:20" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:20" ht="150" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>176</v>
       </c>
@@ -3466,7 +3466,7 @@
       </c>
       <c r="J68" s="5"/>
     </row>
-    <row r="69" spans="1:20" ht="116" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:20" ht="135" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>179</v>
       </c>
@@ -3501,7 +3501,7 @@
       <c r="R69" s="6"/>
       <c r="S69" s="6"/>
     </row>
-    <row r="70" spans="1:20" ht="87" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" ht="105" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>182</v>
       </c>
@@ -3537,7 +3537,7 @@
       <c r="S70" s="5"/>
       <c r="T70"/>
     </row>
-    <row r="71" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>184</v>
       </c>
@@ -3573,7 +3573,7 @@
       <c r="S71" s="5"/>
       <c r="T71" s="5"/>
     </row>
-    <row r="72" spans="1:20" ht="145" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:20" ht="180" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>185</v>
       </c>
@@ -3609,7 +3609,7 @@
       <c r="S72" s="5"/>
       <c r="T72" s="5"/>
     </row>
-    <row r="73" spans="1:20" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:20" ht="135" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>186</v>
       </c>
@@ -3645,7 +3645,7 @@
       <c r="S73" s="5"/>
       <c r="T73" s="5"/>
     </row>
-    <row r="74" spans="1:20" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:20" ht="180" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>188</v>
       </c>
@@ -3681,7 +3681,7 @@
       <c r="S74" s="5"/>
       <c r="T74" s="5"/>
     </row>
-    <row r="75" spans="1:20" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:20" ht="180" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>189</v>
       </c>
@@ -3717,7 +3717,7 @@
       <c r="S75" s="5"/>
       <c r="T75" s="5"/>
     </row>
-    <row r="76" spans="1:20" ht="116" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:20" ht="135" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>191</v>
       </c>
@@ -3753,7 +3753,7 @@
       <c r="S76" s="5"/>
       <c r="T76" s="5"/>
     </row>
-    <row r="77" spans="1:20" ht="174" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:20" ht="210" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>192</v>
       </c>
@@ -3789,7 +3789,7 @@
       <c r="S77" s="5"/>
       <c r="T77" s="5"/>
     </row>
-    <row r="78" spans="1:20" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:20" ht="165" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>193</v>
       </c>
@@ -3825,7 +3825,7 @@
       <c r="S78" s="5"/>
       <c r="T78" s="5"/>
     </row>
-    <row r="79" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>202</v>
       </c>
@@ -3861,7 +3861,7 @@
       <c r="S79" s="5"/>
       <c r="T79" s="5"/>
     </row>
-    <row r="80" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>206</v>
       </c>
@@ -3897,7 +3897,7 @@
       <c r="S80" s="5"/>
       <c r="T80" s="5"/>
     </row>
-    <row r="81" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>207</v>
       </c>
@@ -3933,7 +3933,7 @@
       <c r="S81" s="5"/>
       <c r="T81" s="5"/>
     </row>
-    <row r="82" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>208</v>
       </c>
@@ -3969,7 +3969,7 @@
       <c r="S82" s="5"/>
       <c r="T82" s="5"/>
     </row>
-    <row r="83" spans="1:20" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:20" ht="120" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>209</v>
       </c>
@@ -4005,7 +4005,7 @@
       <c r="S83" s="5"/>
       <c r="T83" s="5"/>
     </row>
-    <row r="84" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>211</v>
       </c>
@@ -4040,7 +4040,7 @@
       <c r="R84" s="5"/>
       <c r="S84" s="5"/>
     </row>
-    <row r="85" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>214</v>
       </c>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="J85" s="5"/>
     </row>
-    <row r="86" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>215</v>
       </c>
@@ -4094,7 +4094,7 @@
       </c>
       <c r="J86" s="5"/>
     </row>
-    <row r="87" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>216</v>
       </c>
@@ -4121,7 +4121,7 @@
       </c>
       <c r="J87" s="5"/>
     </row>
-    <row r="88" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>219</v>
       </c>
@@ -4148,7 +4148,7 @@
       </c>
       <c r="J88" s="5"/>
     </row>
-    <row r="89" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>224</v>
       </c>
@@ -4175,7 +4175,7 @@
       </c>
       <c r="J89" s="5"/>
     </row>
-    <row r="90" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>225</v>
       </c>
@@ -4202,7 +4202,7 @@
       </c>
       <c r="J90" s="5"/>
     </row>
-    <row r="91" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>227</v>
       </c>
@@ -4229,7 +4229,7 @@
       </c>
       <c r="J91" s="5"/>
     </row>
-    <row r="92" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>229</v>
       </c>
@@ -4256,7 +4256,7 @@
       </c>
       <c r="J92" s="5"/>
     </row>
-    <row r="93" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>231</v>
       </c>
@@ -4283,7 +4283,7 @@
       </c>
       <c r="J93" s="5"/>
     </row>
-    <row r="94" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>233</v>
       </c>
@@ -4310,7 +4310,7 @@
       </c>
       <c r="J94" s="5"/>
     </row>
-    <row r="95" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>235</v>
       </c>
@@ -4337,7 +4337,7 @@
       </c>
       <c r="J95" s="5"/>
     </row>
-    <row r="96" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>238</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>237</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>321</v>
+        <v>149</v>
       </c>
       <c r="F96" s="5">
         <v>12</v>
@@ -4364,7 +4364,7 @@
       </c>
       <c r="J96" s="5"/>
     </row>
-    <row r="97" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>240</v>
       </c>
@@ -4391,7 +4391,7 @@
       </c>
       <c r="J97" s="5"/>
     </row>
-    <row r="98" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>242</v>
       </c>
@@ -4418,7 +4418,7 @@
       </c>
       <c r="J98" s="5"/>
     </row>
-    <row r="99" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>244</v>
       </c>
@@ -4444,7 +4444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>246</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>248</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>250</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>252</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>255</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>257</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>259</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>262</v>
       </c>
@@ -4652,7 +4652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>265</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>268</v>
       </c>
@@ -4704,7 +4704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>270</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>271</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>274</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>277</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>280</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>281</v>
       </c>
@@ -4860,7 +4860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>282</v>
       </c>
@@ -4886,7 +4886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>285</v>
       </c>
@@ -4912,7 +4912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>286</v>
       </c>
@@ -4938,424 +4938,424 @@
         <v>149</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="4"/>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="4"/>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="4"/>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="4"/>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="4"/>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="4"/>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="4"/>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
       <c r="B151" s="4"/>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
       <c r="B152" s="4"/>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
       <c r="B153" s="4"/>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
       <c r="B154" s="4"/>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
       <c r="B155" s="4"/>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
       <c r="B156" s="4"/>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2"/>
       <c r="B157" s="4"/>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
       <c r="B158" s="4"/>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
       <c r="B159" s="4"/>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
       <c r="B160" s="4"/>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="4"/>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162" s="4"/>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="4"/>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="4"/>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165" s="4"/>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
       <c r="B166" s="4"/>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
       <c r="B167" s="4"/>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="4"/>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
       <c r="B169" s="4"/>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170" s="4"/>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171" s="4"/>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172" s="4"/>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173" s="4"/>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174" s="4"/>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="4"/>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176" s="4"/>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
       <c r="B177" s="4"/>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
       <c r="B178" s="4"/>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179" s="4"/>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
       <c r="B180" s="4"/>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
       <c r="B181" s="4"/>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
       <c r="B182" s="4"/>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
       <c r="B183" s="4"/>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
       <c r="B184" s="4"/>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
       <c r="B185" s="4"/>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
       <c r="B186" s="4"/>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
       <c r="B187" s="4"/>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
       <c r="B188" s="4"/>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
       <c r="B189" s="4"/>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
       <c r="B190" s="4"/>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
       <c r="B191" s="4"/>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
       <c r="B192" s="4"/>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="2"/>
       <c r="B193" s="4"/>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
       <c r="B194" s="4"/>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="2"/>
       <c r="B195" s="4"/>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="2"/>
       <c r="B196" s="4"/>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
       <c r="B197" s="4"/>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
       <c r="B198" s="4"/>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
       <c r="B199" s="4"/>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="2"/>
       <c r="B200" s="4"/>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B201" s="4"/>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B202" s="4"/>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B203" s="4"/>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B204" s="4"/>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B205" s="4"/>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B206" s="4"/>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B207" s="4"/>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B208" s="4"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B209" s="4"/>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B210" s="4"/>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B211" s="4"/>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B212" s="4"/>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B213" s="4"/>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B214" s="4"/>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B215" s="4"/>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B216" s="4"/>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B217" s="4"/>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B218" s="4"/>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B219" s="4"/>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B220" s="4"/>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B221" s="4"/>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B222" s="4"/>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B223" s="4"/>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B224" s="4"/>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B225" s="4"/>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B226" s="4"/>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B227" s="4"/>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B228" s="4"/>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B229" s="4"/>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B230" s="4"/>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B231" s="4"/>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B232" s="4"/>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B233" s="4"/>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B234" s="4"/>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B235" s="4"/>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B236" s="4"/>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B237" s="4"/>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B238" s="4"/>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B239" s="4"/>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B240" s="4"/>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B241" s="4"/>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B242" s="4"/>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B243" s="4"/>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B244" s="4"/>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B245" s="4"/>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B246" s="4"/>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B247" s="4"/>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B248" s="4"/>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B249" s="4"/>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B250" s="4"/>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B251" s="4"/>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B252" s="4"/>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B253" s="4"/>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B254" s="4"/>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B255" s="4"/>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B256" s="4"/>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B257" s="4"/>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B258" s="4"/>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B259" s="4"/>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B260" s="4"/>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="261" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B261" s="4"/>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="262" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B262" s="4"/>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="263" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B263" s="4"/>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="264" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B264" s="4"/>
     </row>
   </sheetData>

</xml_diff>